<commit_message>
This file now has the full list of TetR orthologs I want to add to this collection
</commit_message>
<xml_diff>
--- a/tetR Orthologs/tetR Orthologs.xlsx
+++ b/tetR Orthologs/tetR Orthologs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracihaddock/Git/iGEM-distribution/tetR Orthologs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79505F28-A77F-3C45-AD49-905840C88290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EE3340-342D-7D43-8995-D8FCB43DDEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="34060" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="500" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,19 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ontology Terms'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Organism Terms'!$A$1:$B$1000</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataSignature="AMtx7miW6g6zRmueViZFkusAasilJg/+wQ=="/>
     </ext>
@@ -34,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7546" uniqueCount="7516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7617" uniqueCount="7549">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22643,12 +22653,111 @@
   <si>
     <t>DNA Parts and Devices</t>
   </si>
+  <si>
+    <t>LmrA</t>
+  </si>
+  <si>
+    <t>AmtR</t>
+  </si>
+  <si>
+    <t>SrpR</t>
+  </si>
+  <si>
+    <t>TarA</t>
+  </si>
+  <si>
+    <t>QacR</t>
+  </si>
+  <si>
+    <t>IcaR(A)</t>
+  </si>
+  <si>
+    <t>ScbR</t>
+  </si>
+  <si>
+    <t>ButR</t>
+  </si>
+  <si>
+    <t>PhlF</t>
+  </si>
+  <si>
+    <t>SmcR</t>
+  </si>
+  <si>
+    <t>McbR</t>
+  </si>
+  <si>
+    <t>PsrA</t>
+  </si>
+  <si>
+    <t>BetI</t>
+  </si>
+  <si>
+    <t>LitR</t>
+  </si>
+  <si>
+    <t>Orf2</t>
+  </si>
+  <si>
+    <t>HapR</t>
+  </si>
+  <si>
+    <t>HlyllR</t>
+  </si>
+  <si>
+    <t>AmeR</t>
+  </si>
+  <si>
+    <t>BM3R1</t>
+  </si>
+  <si>
+    <t>Bacillus subtilis</t>
+  </si>
+  <si>
+    <t>Pseudomonas putida</t>
+  </si>
+  <si>
+    <t>Streptomyces tendae</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus</t>
+  </si>
+  <si>
+    <t>Streptomyces coelicolor</t>
+  </si>
+  <si>
+    <t>Streptomyces cinnamonensis</t>
+  </si>
+  <si>
+    <t>Pseudomonas fluorescens</t>
+  </si>
+  <si>
+    <t>Vibrio vulnificus</t>
+  </si>
+  <si>
+    <t>Vibrio fischeri</t>
+  </si>
+  <si>
+    <t>Streptomyces griseus</t>
+  </si>
+  <si>
+    <t>Vibrio cholerae</t>
+  </si>
+  <si>
+    <t>Bacillus cereus</t>
+  </si>
+  <si>
+    <t>Agrobacterium tumefaciens</t>
+  </si>
+  <si>
+    <t>Bacillus megaterium</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -22840,6 +22949,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -22988,7 +23102,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23047,6 +23161,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23503,8 +23623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23824,15 +23944,21 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A15" s="18"/>
+      <c r="A15" s="18" t="s">
+        <v>7516</v>
+      </c>
       <c r="B15" s="43"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="H15" s="18" t="s">
+        <v>7535</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J15" s="18" t="b">
         <v>0</v>
       </c>
@@ -23846,15 +23972,21 @@
       <c r="M15" s="20"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A16" s="22"/>
+      <c r="A16" s="22" t="s">
+        <v>7517</v>
+      </c>
       <c r="B16" s="18"/>
       <c r="C16" s="22"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="H16" s="18" t="s">
+        <v>7443</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J16" s="22" t="b">
         <v>0</v>
       </c>
@@ -23868,15 +24000,21 @@
       <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="18"/>
+      <c r="A17" s="18" t="s">
+        <v>7518</v>
+      </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="H17" s="18" t="s">
+        <v>7536</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J17" s="18" t="b">
         <v>0</v>
       </c>
@@ -23890,15 +24028,21 @@
       <c r="M17" s="24"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="18"/>
+      <c r="A18" s="18" t="s">
+        <v>7519</v>
+      </c>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="21"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="H18" s="18" t="s">
+        <v>7537</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J18" s="18" t="b">
         <v>0</v>
       </c>
@@ -23912,15 +24056,21 @@
       <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="18"/>
+      <c r="A19" s="18" t="s">
+        <v>7520</v>
+      </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="21"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="21"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="H19" s="18" t="s">
+        <v>7538</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J19" s="18" t="b">
         <v>0</v>
       </c>
@@ -23934,15 +24084,21 @@
       <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="18"/>
+      <c r="A20" s="18" t="s">
+        <v>7521</v>
+      </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="D20" s="21"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="21"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="H20" s="18" t="s">
+        <v>7538</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J20" s="18" t="b">
         <v>0</v>
       </c>
@@ -23956,15 +24112,21 @@
       <c r="M20" s="22"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="18"/>
+      <c r="A21" s="18" t="s">
+        <v>7522</v>
+      </c>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
       <c r="D21" s="21"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="H21" s="18" t="s">
+        <v>7539</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J21" s="18" t="b">
         <v>0</v>
       </c>
@@ -23978,15 +24140,21 @@
       <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="18"/>
+      <c r="A22" s="18" t="s">
+        <v>7523</v>
+      </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
+      <c r="H22" s="18" t="s">
+        <v>7540</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J22" s="18" t="b">
         <v>0</v>
       </c>
@@ -24000,15 +24168,21 @@
       <c r="M22" s="18"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="18"/>
+      <c r="A23" s="18" t="s">
+        <v>7524</v>
+      </c>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
+      <c r="H23" s="18" t="s">
+        <v>7541</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J23" s="18" t="b">
         <v>0</v>
       </c>
@@ -24022,15 +24196,21 @@
       <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="18"/>
+      <c r="A24" s="18" t="s">
+        <v>7525</v>
+      </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
       <c r="D24" s="21"/>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="21"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="H24" s="18" t="s">
+        <v>7542</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J24" s="18" t="b">
         <v>0</v>
       </c>
@@ -24044,15 +24224,21 @@
       <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A25" s="18"/>
+      <c r="A25" s="18" t="s">
+        <v>7526</v>
+      </c>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
       <c r="D25" s="21"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
+      <c r="H25" s="18" t="s">
+        <v>7443</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J25" s="18" t="b">
         <v>0</v>
       </c>
@@ -24066,15 +24252,21 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A26" s="18"/>
+      <c r="A26" s="18" t="s">
+        <v>7527</v>
+      </c>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+      <c r="H26" s="18" t="s">
+        <v>7536</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J26" s="18" t="b">
         <v>0</v>
       </c>
@@ -24088,15 +24280,21 @@
       <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="18"/>
+      <c r="A27" s="18" t="s">
+        <v>7528</v>
+      </c>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
       <c r="D27" s="21"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
+      <c r="H27" s="18" t="s">
+        <v>7419</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J27" s="18" t="b">
         <v>0</v>
       </c>
@@ -24110,15 +24308,21 @@
       <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="43"/>
+      <c r="A28" s="43" t="s">
+        <v>7529</v>
+      </c>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="21"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
+      <c r="H28" s="18" t="s">
+        <v>7543</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J28" s="18" t="b">
         <v>0</v>
       </c>
@@ -24132,15 +24336,21 @@
       <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="43"/>
+      <c r="A29" s="43" t="s">
+        <v>7530</v>
+      </c>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="21"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+      <c r="H29" s="18" t="s">
+        <v>7544</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J29" s="18" t="b">
         <v>0</v>
       </c>
@@ -24154,15 +24364,21 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="43"/>
+      <c r="A30" s="43" t="s">
+        <v>7531</v>
+      </c>
       <c r="B30" s="18"/>
       <c r="C30" s="22"/>
       <c r="D30" s="21"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="21"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="H30" s="18" t="s">
+        <v>7545</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J30" s="18" t="b">
         <v>0</v>
       </c>
@@ -24176,15 +24392,21 @@
       <c r="M30" s="25"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="43"/>
+      <c r="A31" s="43" t="s">
+        <v>7532</v>
+      </c>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="21"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
       <c r="G31" s="21"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="H31" s="18" t="s">
+        <v>7546</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J31" s="18" t="b">
         <v>0</v>
       </c>
@@ -24198,15 +24420,21 @@
       <c r="M31" s="25"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A32" s="43"/>
+      <c r="A32" s="43" t="s">
+        <v>7533</v>
+      </c>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
       <c r="D32" s="21"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="21"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
+      <c r="H32" s="18" t="s">
+        <v>7547</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J32" s="18" t="b">
         <v>0</v>
       </c>
@@ -24220,15 +24448,21 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A33" s="43"/>
+      <c r="A33" s="43" t="s">
+        <v>7534</v>
+      </c>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
       <c r="D33" s="21"/>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="21"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
+      <c r="H33" s="18" t="s">
+        <v>7548</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J33" s="18" t="b">
         <v>0</v>
       </c>
@@ -24242,7 +24476,6 @@
       <c r="M33" s="26"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A34" s="43"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
       <c r="D34" s="21"/>
@@ -25307,7 +25540,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$11</xm:f>
@@ -25318,7 +25551,7 @@
           <x14:formula1>
             <xm:f>'Organism Terms'!$A$2:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>H15:I38</xm:sqref>
+          <xm:sqref>I15:I38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -25337,6 +25570,12 @@
             <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>J15:K38</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{0E82918C-B909-714A-937A-FBEFE5F8D328}">
+          <x14:formula1>
+            <xm:f>'Organism Terms'!$A$2:$A$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>H15 H16:H38</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -68616,13 +68855,13 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
@@ -68652,11 +68891,11 @@
       <c r="V1" s="3"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>7417</v>
+      <c r="A2" s="21" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="3">
-        <v>32630</v>
+        <v>6100</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -68674,12 +68913,10 @@
       <c r="V2" s="3"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>7418</v>
-      </c>
-      <c r="B3" s="3">
-        <v>4932</v>
-      </c>
+      <c r="A3" s="51" t="s">
+        <v>7547</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -68695,11 +68932,11 @@
       <c r="V3" s="3"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>7419</v>
-      </c>
-      <c r="B4" s="3">
-        <v>562</v>
+      <c r="A4" s="43" t="s">
+        <v>7442</v>
+      </c>
+      <c r="B4" s="18">
+        <v>1034331</v>
       </c>
       <c r="C4" s="3"/>
       <c r="K4" s="3"/>
@@ -68716,11 +68953,11 @@
       <c r="V4" s="3"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>7420</v>
+      <c r="A5" s="21" t="s">
+        <v>7421</v>
       </c>
       <c r="B5" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3"/>
       <c r="K5" s="3"/>
@@ -68737,11 +68974,11 @@
       <c r="V5" s="3"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>7421</v>
-      </c>
-      <c r="B6" s="6">
-        <v>6</v>
+      <c r="A6" s="21" t="s">
+        <v>7422</v>
+      </c>
+      <c r="B6" s="21">
+        <v>7</v>
       </c>
       <c r="C6" s="3"/>
       <c r="K6" s="3"/>
@@ -68758,12 +68995,10 @@
       <c r="V6" s="3"/>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>7422</v>
-      </c>
-      <c r="B7" s="6">
-        <v>7</v>
-      </c>
+      <c r="A7" s="53" t="s">
+        <v>7546</v>
+      </c>
+      <c r="B7" s="18"/>
       <c r="C7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -68779,12 +69014,10 @@
       <c r="V7" s="3"/>
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>7423</v>
-      </c>
-      <c r="B8" s="6">
-        <v>9</v>
-      </c>
+      <c r="A8" s="51" t="s">
+        <v>7548</v>
+      </c>
+      <c r="B8" s="18"/>
       <c r="C8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -68800,12 +69033,10 @@
       <c r="V8" s="3"/>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>7424</v>
-      </c>
-      <c r="B9" s="3">
-        <v>10</v>
-      </c>
+      <c r="A9" s="50" t="s">
+        <v>7535</v>
+      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -68821,11 +69052,11 @@
       <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A10" s="6" t="s">
-        <v>7425</v>
-      </c>
-      <c r="B10" s="3">
-        <v>11</v>
+      <c r="A10" s="21" t="s">
+        <v>7420</v>
+      </c>
+      <c r="B10" s="21">
+        <v>2</v>
       </c>
       <c r="C10" s="3"/>
       <c r="K10" s="3"/>
@@ -68842,11 +69073,11 @@
       <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A11" s="6" t="s">
-        <v>7426</v>
-      </c>
-      <c r="B11" s="3">
-        <v>12</v>
+      <c r="A11" s="21" t="s">
+        <v>7423</v>
+      </c>
+      <c r="B11" s="21">
+        <v>9</v>
       </c>
       <c r="C11" s="3"/>
       <c r="K11" s="3"/>
@@ -68863,240 +69094,290 @@
       <c r="V11" s="3"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="21" t="s">
+        <v>7425</v>
+      </c>
+      <c r="B12" s="3">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A13" s="21" t="s">
+        <v>7424</v>
+      </c>
+      <c r="B13" s="3">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A14" s="21" t="s">
+        <v>7443</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1718</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A15" s="21" t="s">
         <v>7427</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B15" s="3">
         <v>13</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A16" s="21" t="s">
         <v>7428</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B16" s="3">
         <v>14</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A14" s="6" t="s">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A17" s="43" t="s">
+        <v>7419</v>
+      </c>
+      <c r="B17" s="3">
+        <v>562</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A18" s="21" t="s">
+        <v>7440</v>
+      </c>
+      <c r="B18" s="3">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A19" s="21" t="s">
+        <v>7439</v>
+      </c>
+      <c r="B19" s="3">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A20" s="21" t="s">
         <v>7429</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B20" s="3">
         <v>16</v>
       </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A15" s="6" t="s">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A21" s="21" t="s">
         <v>7430</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B21" s="3">
         <v>17</v>
       </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A16" s="6" t="s">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A22" s="21" t="s">
+        <v>7441</v>
+      </c>
+      <c r="B22" s="3">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A23" s="21" t="s">
         <v>7431</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B23" s="3">
         <v>18</v>
       </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A24" s="21" t="s">
         <v>7432</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B24" s="3">
         <v>19</v>
       </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A18" s="6" t="s">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A25" s="21" t="s">
         <v>7433</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B25" s="3">
         <v>20</v>
       </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="6" t="s">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A26" s="21" t="s">
         <v>7434</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B26" s="3">
         <v>21</v>
       </c>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="6" t="s">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A27" s="21" t="s">
+        <v>7426</v>
+      </c>
+      <c r="B27" s="3">
+        <v>12</v>
+      </c>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A28" s="50" t="s">
+        <v>7541</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A29" s="50" t="s">
+        <v>7536</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A30" s="43" t="s">
+        <v>7418</v>
+      </c>
+      <c r="B30" s="3">
+        <v>4932</v>
+      </c>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A31" s="21" t="s">
         <v>7435</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B31" s="3">
         <v>22</v>
       </c>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="6" t="s">
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" ht="15" customHeight="1">
+      <c r="A32" s="21" t="s">
         <v>7436</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B32" s="3">
         <v>23</v>
       </c>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="6" t="s">
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A33" s="21" t="s">
+        <v>7438</v>
+      </c>
+      <c r="B33" s="3">
+        <v>25</v>
+      </c>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A34" s="21" t="s">
         <v>7437</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B34" s="3">
         <v>24</v>
       </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="6" t="s">
-        <v>7438</v>
-      </c>
-      <c r="B23" s="3">
-        <v>25</v>
-      </c>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="6" t="s">
-        <v>7439</v>
-      </c>
-      <c r="B24" s="3">
-        <v>27</v>
-      </c>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="6" t="s">
-        <v>7440</v>
-      </c>
-      <c r="B25" s="3">
-        <v>28</v>
-      </c>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="6" t="s">
-        <v>7441</v>
-      </c>
-      <c r="B26" s="3">
-        <v>29</v>
-      </c>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="3" t="s">
-        <v>7442</v>
-      </c>
-      <c r="B27" s="3">
-        <v>1034331</v>
-      </c>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28" s="6" t="s">
-        <v>7443</v>
-      </c>
-      <c r="B28" s="3">
-        <v>1718</v>
-      </c>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A29" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="3">
-        <v>6100</v>
-      </c>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A35" s="50" t="s">
+        <v>7538</v>
+      </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="2:3" ht="15.75" customHeight="1">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A36" s="50" t="s">
+        <v>7540</v>
+      </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="2:3" ht="15.75" customHeight="1">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A37" s="50" t="s">
+        <v>7539</v>
+      </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="2:3" ht="15.75" customHeight="1">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A38" s="50" t="s">
+        <v>7544</v>
+      </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="2:3" ht="15.75" customHeight="1">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A39" s="50" t="s">
+        <v>7537</v>
+      </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B40" s="3"/>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A40" s="43" t="s">
+        <v>7417</v>
+      </c>
+      <c r="B40" s="3">
+        <v>32630</v>
+      </c>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="2:3" ht="15.75" customHeight="1">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A41" s="52" t="s">
+        <v>7545</v>
+      </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="2:3" ht="15.75" customHeight="1">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A42" s="52" t="s">
+        <v>7543</v>
+      </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="2:3" ht="15.75" customHeight="1">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A43" s="52" t="s">
+        <v>7542</v>
+      </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="2:3" ht="15.75" customHeight="1">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="2:3" ht="15.75" customHeight="1">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="2:3" ht="15.75" customHeight="1">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="2:3" ht="15.75" customHeight="1">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="2:3" ht="15.75" customHeight="1">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
@@ -70596,6 +70877,11 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <autoFilter ref="A1:B1000" xr:uid="{18AB4AFC-BFF3-6E40-B6ED-F89E24D4773C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B1000">
+      <sortCondition ref="A1:A1000"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
Work in progress: additions to the TetR Orthologs spreadsheet
</commit_message>
<xml_diff>
--- a/tetR Orthologs/tetR Orthologs.xlsx
+++ b/tetR Orthologs/tetR Orthologs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracihaddock/Git/iGEM-distribution/tetR Orthologs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EE3340-342D-7D43-8995-D8FCB43DDEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96965FA4-8AF1-D146-ADA8-2691DEFE9FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="500" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28260" yWindow="500" windowWidth="37440" windowHeight="23840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7617" uniqueCount="7549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7680" uniqueCount="7581">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22669,9 +22669,6 @@
     <t>QacR</t>
   </si>
   <si>
-    <t>IcaR(A)</t>
-  </si>
-  <si>
     <t>ScbR</t>
   </si>
   <si>
@@ -22751,13 +22748,112 @@
   </si>
   <si>
     <t>Bacillus megaterium</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Cello_Parts/AmtR/1</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/LmrA/1</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/SrpR/1</t>
+  </si>
+  <si>
+    <t>not in SynBioHub</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/QacR/1</t>
+  </si>
+  <si>
+    <t>pQacR</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/pQacR/1</t>
+  </si>
+  <si>
+    <t>pAmtR</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/pAmtR/1</t>
+  </si>
+  <si>
+    <t>pSrpR</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/pSrpR/1</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/IcaRA/1</t>
+  </si>
+  <si>
+    <t>IcaRA</t>
+  </si>
+  <si>
+    <t>pIcaRA</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/pIcaRA/1</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/PhlF/1</t>
+  </si>
+  <si>
+    <t>pPhlF</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/pPhlF/1</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/PsrA/1</t>
+  </si>
+  <si>
+    <t>pPsrA</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/pPsrA/1</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/BetI/1</t>
+  </si>
+  <si>
+    <t>pBetI</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/pBetI/1</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/LitR/1</t>
+  </si>
+  <si>
+    <t>pLitR</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/pLitR/1</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/AmeR/1</t>
+  </si>
+  <si>
+    <t>pAmeR</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/pAmeR/1</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/BM3R1/1</t>
+  </si>
+  <si>
+    <t>pBM3R1</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/pBM3R1/1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="30">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -22835,21 +22931,8 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Lato"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -22955,7 +23038,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -22974,8 +23057,20 @@
         <bgColor rgb="FFE2EFD9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor theme="9" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -23097,12 +23192,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23122,40 +23232,36 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -23164,9 +23270,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23623,8 +23737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23656,7 +23770,7 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2"/>
@@ -23694,12 +23808,12 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="47"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -23736,7 +23850,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" s="22" customFormat="1" ht="15.75" customHeight="1">
+    <row r="8" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="12" t="s">
         <v>7506</v>
       </c>
@@ -23862,7 +23976,7 @@
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="41" t="s">
         <v>7512</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -23947,14 +24061,16 @@
       <c r="A15" s="18" t="s">
         <v>7516</v>
       </c>
-      <c r="B15" s="43"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
+      <c r="G15" s="55" t="s">
+        <v>7549</v>
+      </c>
       <c r="H15" s="18" t="s">
-        <v>7535</v>
+        <v>7534</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>7419</v>
@@ -23966,31 +24082,33 @@
         <v>0</v>
       </c>
       <c r="L15" s="15">
-        <f t="shared" ref="L15:L38" si="0">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M15,CHAR(160)," ")," ",""))))</f>
+        <f t="shared" ref="L15:L37" si="0">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M15,CHAR(160)," ")," ",""))))</f>
         <v>0</v>
       </c>
-      <c r="M15" s="20"/>
+      <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>7517</v>
       </c>
       <c r="B16" s="18"/>
-      <c r="C16" s="22"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="54" t="s">
+        <v>7548</v>
+      </c>
       <c r="H16" s="18" t="s">
         <v>7443</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>7419</v>
       </c>
-      <c r="J16" s="22" t="b">
+      <c r="J16" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="K16" s="22" t="b">
+      <c r="K16" s="21" t="b">
         <v>0</v>
       </c>
       <c r="L16" s="15">
@@ -24008,9 +24126,11 @@
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="G17" s="56" t="s">
+        <v>7550</v>
+      </c>
       <c r="H17" s="18" t="s">
-        <v>7536</v>
+        <v>7535</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>7419</v>
@@ -24025,20 +24145,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M17" s="24"/>
+      <c r="M17" s="22"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="18" t="s">
         <v>7519</v>
       </c>
       <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="41" t="s">
+        <v>7551</v>
+      </c>
+      <c r="D18" s="20"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
       <c r="H18" s="18" t="s">
-        <v>7537</v>
+        <v>7536</v>
       </c>
       <c r="I18" s="18" t="s">
         <v>7419</v>
@@ -24061,12 +24183,14 @@
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
-      <c r="D19" s="21"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
-      <c r="G19" s="21"/>
+      <c r="G19" s="56" t="s">
+        <v>7552</v>
+      </c>
       <c r="H19" s="18" t="s">
-        <v>7538</v>
+        <v>7537</v>
       </c>
       <c r="I19" s="18" t="s">
         <v>7419</v>
@@ -24084,17 +24208,19 @@
       <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="18" t="s">
-        <v>7521</v>
+      <c r="A20" s="41" t="s">
+        <v>7560</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
-      <c r="D20" s="21"/>
+      <c r="D20" s="20"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
-      <c r="G20" s="21"/>
+      <c r="G20" s="20" t="s">
+        <v>7559</v>
+      </c>
       <c r="H20" s="18" t="s">
-        <v>7538</v>
+        <v>7537</v>
       </c>
       <c r="I20" s="18" t="s">
         <v>7419</v>
@@ -24109,20 +24235,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M20" s="22"/>
+      <c r="M20" s="21"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="18" t="s">
-        <v>7522</v>
+      <c r="A21" s="41" t="s">
+        <v>7521</v>
       </c>
       <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="21"/>
+      <c r="C21" s="41" t="s">
+        <v>7551</v>
+      </c>
+      <c r="D21" s="20"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18" t="s">
-        <v>7539</v>
+        <v>7538</v>
       </c>
       <c r="I21" s="18" t="s">
         <v>7419</v>
@@ -24141,16 +24269,18 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>7523</v>
+        <v>7522</v>
       </c>
       <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
+      <c r="C22" s="41" t="s">
+        <v>7551</v>
+      </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
       <c r="H22" s="18" t="s">
-        <v>7540</v>
+        <v>7539</v>
       </c>
       <c r="I22" s="18" t="s">
         <v>7419</v>
@@ -24169,16 +24299,18 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>7524</v>
+        <v>7523</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="G23" s="18" t="s">
+        <v>7563</v>
+      </c>
       <c r="H23" s="18" t="s">
-        <v>7541</v>
+        <v>7540</v>
       </c>
       <c r="I23" s="18" t="s">
         <v>7419</v>
@@ -24196,17 +24328,19 @@
       <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="18" t="s">
-        <v>7525</v>
+      <c r="A24" s="41" t="s">
+        <v>7524</v>
       </c>
       <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="21"/>
+      <c r="C24" s="41" t="s">
+        <v>7551</v>
+      </c>
+      <c r="D24" s="20"/>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
-      <c r="G24" s="21"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="18" t="s">
-        <v>7542</v>
+        <v>7541</v>
       </c>
       <c r="I24" s="18" t="s">
         <v>7419</v>
@@ -24225,14 +24359,16 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>7526</v>
+        <v>7525</v>
       </c>
       <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="21"/>
+      <c r="C25" s="41" t="s">
+        <v>7551</v>
+      </c>
+      <c r="D25" s="20"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
-      <c r="G25" s="21"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="18" t="s">
         <v>7443</v>
       </c>
@@ -24253,16 +24389,18 @@
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>7527</v>
+        <v>7526</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="G26" s="56" t="s">
+        <v>7566</v>
+      </c>
       <c r="H26" s="18" t="s">
-        <v>7536</v>
+        <v>7535</v>
       </c>
       <c r="I26" s="18" t="s">
         <v>7419</v>
@@ -24281,14 +24419,16 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>7528</v>
+        <v>7527</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
-      <c r="D27" s="21"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="G27" s="56" t="s">
+        <v>7569</v>
+      </c>
       <c r="H27" s="18" t="s">
         <v>7419</v>
       </c>
@@ -24308,17 +24448,19 @@
       <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="43" t="s">
-        <v>7529</v>
+      <c r="A28" s="41" t="s">
+        <v>7528</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
-      <c r="D28" s="21"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="G28" s="56" t="s">
+        <v>7572</v>
+      </c>
       <c r="H28" s="18" t="s">
-        <v>7543</v>
+        <v>7542</v>
       </c>
       <c r="I28" s="18" t="s">
         <v>7419</v>
@@ -24336,17 +24478,19 @@
       <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="43" t="s">
-        <v>7530</v>
+      <c r="A29" s="41" t="s">
+        <v>7529</v>
       </c>
       <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="21"/>
+      <c r="C29" s="41" t="s">
+        <v>7551</v>
+      </c>
+      <c r="D29" s="20"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
       <c r="H29" s="18" t="s">
-        <v>7544</v>
+        <v>7543</v>
       </c>
       <c r="I29" s="18" t="s">
         <v>7419</v>
@@ -24364,17 +24508,19 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="43" t="s">
-        <v>7531</v>
+      <c r="A30" s="41" t="s">
+        <v>7530</v>
       </c>
       <c r="B30" s="18"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="21"/>
+      <c r="C30" s="41" t="s">
+        <v>7551</v>
+      </c>
+      <c r="D30" s="20"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="21"/>
+      <c r="G30" s="20"/>
       <c r="H30" s="18" t="s">
-        <v>7545</v>
+        <v>7544</v>
       </c>
       <c r="I30" s="18" t="s">
         <v>7419</v>
@@ -24389,20 +24535,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M30" s="25"/>
+      <c r="M30" s="23"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="43" t="s">
-        <v>7532</v>
+      <c r="A31" s="41" t="s">
+        <v>7531</v>
       </c>
       <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="21"/>
+      <c r="C31" s="41" t="s">
+        <v>7551</v>
+      </c>
+      <c r="D31" s="20"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="21"/>
+      <c r="G31" s="20"/>
       <c r="H31" s="18" t="s">
-        <v>7546</v>
+        <v>7545</v>
       </c>
       <c r="I31" s="18" t="s">
         <v>7419</v>
@@ -24417,20 +24565,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M31" s="25"/>
+      <c r="M31" s="23"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A32" s="43" t="s">
-        <v>7533</v>
+      <c r="A32" s="41" t="s">
+        <v>7532</v>
       </c>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
-      <c r="D32" s="21"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="21"/>
+      <c r="G32" s="56" t="s">
+        <v>7575</v>
+      </c>
       <c r="H32" s="18" t="s">
-        <v>7547</v>
+        <v>7546</v>
       </c>
       <c r="I32" s="18" t="s">
         <v>7419</v>
@@ -24448,17 +24598,19 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A33" s="43" t="s">
-        <v>7534</v>
+      <c r="A33" s="41" t="s">
+        <v>7533</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
-      <c r="D33" s="21"/>
+      <c r="D33" s="20"/>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
-      <c r="G33" s="21"/>
+      <c r="G33" s="56" t="s">
+        <v>7578</v>
+      </c>
       <c r="H33" s="18" t="s">
-        <v>7548</v>
+        <v>7547</v>
       </c>
       <c r="I33" s="18" t="s">
         <v>7419</v>
@@ -24473,15 +24625,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M33" s="26"/>
+      <c r="M33" s="24"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A34" s="53" t="s">
+        <v>7501</v>
+      </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
-      <c r="D34" s="21"/>
+      <c r="D34" s="20"/>
       <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="21"/>
+      <c r="F34" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>7501</v>
+      </c>
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18" t="b">
@@ -24494,16 +24653,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M34" s="22"/>
+      <c r="M34" s="21"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A35" s="43"/>
+      <c r="A35" s="41" t="s">
+        <v>7502</v>
+      </c>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
-      <c r="D35" s="21"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
-      <c r="G35" s="21"/>
+      <c r="G35" s="20"/>
       <c r="H35" s="18"/>
       <c r="I35" s="18"/>
       <c r="J35" s="18" t="b">
@@ -24516,18 +24677,26 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M35" s="22"/>
+      <c r="M35" s="21"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="43"/>
+      <c r="A36" s="41" t="s">
+        <v>7553</v>
+      </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
-      <c r="D36" s="21"/>
+      <c r="D36" s="20"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
+      <c r="G36" s="56" t="s">
+        <v>7554</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>7537</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J36" s="18" t="b">
         <v>0</v>
       </c>
@@ -24538,18 +24707,26 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M36" s="22"/>
+      <c r="M36" s="21"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A37" s="43"/>
+      <c r="A37" s="41" t="s">
+        <v>7555</v>
+      </c>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
-      <c r="D37" s="21"/>
+      <c r="D37" s="20"/>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
+      <c r="G37" s="20" t="s">
+        <v>7556</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>7443</v>
+      </c>
+      <c r="I37" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J37" s="18" t="b">
         <v>0</v>
       </c>
@@ -24560,18 +24737,26 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M37" s="22"/>
+      <c r="M37" s="21"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A38" s="43"/>
+      <c r="A38" s="41" t="s">
+        <v>7557</v>
+      </c>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
-      <c r="D38" s="21"/>
+      <c r="D38" s="20"/>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
+      <c r="G38" s="20" t="s">
+        <v>7558</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>7535</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J38" s="18" t="b">
         <v>0</v>
       </c>
@@ -24579,37 +24764,333 @@
         <v>0</v>
       </c>
       <c r="L38" s="15">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M38,CHAR(160)," ")," ",""))))</f>
         <v>0</v>
       </c>
-      <c r="M38" s="22"/>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="41" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="43" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="44" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="45" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="46" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
+      <c r="M38" s="21"/>
+    </row>
+    <row r="39" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A39" s="41" t="s">
+        <v>7561</v>
+      </c>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="20" t="s">
+        <v>7562</v>
+      </c>
+      <c r="H39" s="52" t="s">
+        <v>7537</v>
+      </c>
+      <c r="I39" s="52" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J39" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L39" s="15">
+        <f t="shared" ref="L39:L40" si="1">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M39,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A40" s="41" t="s">
+        <v>7564</v>
+      </c>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="56" t="s">
+        <v>7565</v>
+      </c>
+      <c r="H40" s="57" t="s">
+        <v>7540</v>
+      </c>
+      <c r="I40" s="57" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J40" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L40" s="15">
+        <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M40,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A41" s="41" t="s">
+        <v>7567</v>
+      </c>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="56" t="s">
+        <v>7568</v>
+      </c>
+      <c r="H41" s="52" t="s">
+        <v>7535</v>
+      </c>
+      <c r="I41" s="52" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J41" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L41" s="15">
+        <f t="shared" ref="L41:L42" si="2">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M41,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A42" s="41" t="s">
+        <v>7570</v>
+      </c>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="56" t="s">
+        <v>7571</v>
+      </c>
+      <c r="H42" s="57" t="s">
+        <v>7419</v>
+      </c>
+      <c r="I42" s="57" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J42" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L42" s="15">
+        <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M42,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A43" s="41" t="s">
+        <v>7573</v>
+      </c>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="56" t="s">
+        <v>7574</v>
+      </c>
+      <c r="H43" s="52" t="s">
+        <v>7542</v>
+      </c>
+      <c r="I43" s="52" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J43" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L43" s="15">
+        <f t="shared" ref="L43:L44" si="3">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M43,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A44" s="41" t="s">
+        <v>7576</v>
+      </c>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="56" t="s">
+        <v>7577</v>
+      </c>
+      <c r="H44" s="52" t="s">
+        <v>7546</v>
+      </c>
+      <c r="I44" s="52" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J44" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L44" s="15">
+        <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M44,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A45" s="41" t="s">
+        <v>7579</v>
+      </c>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="56" t="s">
+        <v>7580</v>
+      </c>
+      <c r="H45" s="57" t="s">
+        <v>7547</v>
+      </c>
+      <c r="I45" s="57" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J45" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L45" s="15">
+        <f t="shared" ref="L45:L46" si="4">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M45,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A46" s="41"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L46" s="15">
+        <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M46,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A47" s="41"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L47" s="15">
+        <f t="shared" ref="L47:L48" si="5">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M47,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A48" s="41"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L48" s="15">
+        <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M48,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A49" s="41"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L49" s="15">
+        <f t="shared" ref="L49:L50" si="6">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M49,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A50" s="41"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L50" s="15">
+        <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M50,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="52" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="53" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="54" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="55" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="56" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="57" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="58" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="59" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="60" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="61" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="62" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="63" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="64" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -25533,10 +26014,28 @@
   <mergeCells count="1">
     <mergeCell ref="A5:F5"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G16" r:id="rId1" xr:uid="{726726F3-6F4A-DB4B-B830-95BCF97F9D9E}"/>
+    <hyperlink ref="G15" r:id="rId2" xr:uid="{5624D566-E4C4-DB45-A4AA-BB2AC3BF50E0}"/>
+    <hyperlink ref="G17" r:id="rId3" xr:uid="{8F9465D5-17F2-FF42-9ACD-2C649CF83E11}"/>
+    <hyperlink ref="G19" r:id="rId4" xr:uid="{C70065B8-A0BE-4649-9563-5E5E5D85EB87}"/>
+    <hyperlink ref="G36" r:id="rId5" xr:uid="{357769C2-1625-D74A-80B1-E075037CBD64}"/>
+    <hyperlink ref="G40" r:id="rId6" xr:uid="{527001D7-7684-C146-9826-04D9AEF8C353}"/>
+    <hyperlink ref="G26" r:id="rId7" xr:uid="{428E1E33-427B-7249-9C7E-0ECDBB554C27}"/>
+    <hyperlink ref="G41" r:id="rId8" xr:uid="{584232BE-CC8C-DC42-8AA1-BD71CBB3B752}"/>
+    <hyperlink ref="G27" r:id="rId9" xr:uid="{48BB666A-0405-5F4F-A70C-B8CC0DC30F7A}"/>
+    <hyperlink ref="G42" r:id="rId10" xr:uid="{7F7F27ED-B36A-EB41-9DAB-31902800C83B}"/>
+    <hyperlink ref="G28" r:id="rId11" xr:uid="{2EBA9145-0113-D44B-A964-D350CECEE260}"/>
+    <hyperlink ref="G43" r:id="rId12" xr:uid="{088F70DF-0573-4F4D-A6F3-936DD4432F82}"/>
+    <hyperlink ref="G32" r:id="rId13" xr:uid="{F6493A6D-D3EE-C843-9EA5-9B4E9F73DC1D}"/>
+    <hyperlink ref="G44" r:id="rId14" xr:uid="{DAF6E551-6F9D-D044-9AE2-23760AE41E3D}"/>
+    <hyperlink ref="G33" r:id="rId15" xr:uid="{38243E19-8216-9446-8B60-4C042B14C971}"/>
+    <hyperlink ref="G45" r:id="rId16" xr:uid="{73B69518-BD7D-554E-9756-E4CBB2D815B4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -25545,37 +26044,37 @@
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F38</xm:sqref>
+          <xm:sqref>F15:F50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Organism Terms'!$A$2:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>I15:I38</xm:sqref>
+          <xm:sqref>I15:I50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'Ontology Terms'!$B$2:$B$2518</xm:f>
           </x14:formula1>
-          <xm:sqref>B15:B38</xm:sqref>
+          <xm:sqref>B15:B50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Sequence_alteration_terms!$A$2:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>D15:D38</xm:sqref>
+          <xm:sqref>D15:D50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J15:K38</xm:sqref>
+          <xm:sqref>J15:K50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{0E82918C-B909-714A-937A-FBEFE5F8D328}">
           <x14:formula1>
             <xm:f>'Organism Terms'!$A$2:$A$50</xm:f>
           </x14:formula1>
-          <xm:sqref>H15 H16:H38</xm:sqref>
+          <xm:sqref>H15:H50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -25588,7 +26087,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -25642,15 +26141,15 @@
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -25664,7 +26163,7 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
     </row>
-    <row r="3" spans="1:26" s="22" customFormat="1" ht="16">
+    <row r="3" spans="1:26" s="21" customFormat="1" ht="16">
       <c r="A3" s="12" t="s">
         <v>7500</v>
       </c>
@@ -25685,9 +26184,9 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
@@ -25724,9 +26223,9 @@
         <v>51</v>
       </c>
       <c r="J4" s="12"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -25763,9 +26262,9 @@
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -25798,9 +26297,9 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -25841,9 +26340,9 @@
       <c r="J7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="31"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="29"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -25878,9 +26377,9 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="31"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="29"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -25984,7 +26483,7 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="41" t="s">
         <v>7512</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -26037,37 +26536,37 @@
       <c r="D13" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="30" t="s">
         <v>73</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="32" t="s">
+      <c r="I13" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="K13" s="32" t="s">
+      <c r="K13" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="L13" s="33" t="s">
+      <c r="L13" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="M13" s="33" t="s">
+      <c r="M13" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="N13" s="33" t="s">
+      <c r="N13" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="O13" s="33" t="s">
+      <c r="O13" s="31" t="s">
         <v>82</v>
       </c>
       <c r="P13" s="3"/>
@@ -26081,16 +26580,16 @@
       <c r="X13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="D14" s="22" t="b">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="D14" s="21" t="b">
         <v>0</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
-      <c r="G14" s="22"/>
+      <c r="G14" s="21"/>
       <c r="H14" s="18"/>
-      <c r="I14" s="34"/>
+      <c r="I14" s="32"/>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -26108,8 +26607,8 @@
       <c r="X14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="16">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="b">
         <v>0</v>
@@ -26117,10 +26616,10 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
-      <c r="H15" s="22"/>
+      <c r="H15" s="21"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
-      <c r="K15" s="21"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="18"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
@@ -26136,17 +26635,17 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
-      <c r="A16" s="22"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
-      <c r="D16" s="22" t="b">
+      <c r="D16" s="21" t="b">
         <v>0</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="22"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="18"/>
-      <c r="I16" s="34"/>
+      <c r="I16" s="32"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -26164,17 +26663,17 @@
       <c r="X16" s="3"/>
     </row>
     <row r="17" spans="1:25" ht="15" customHeight="1">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42" t="b">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="18"/>
-      <c r="I17" s="34"/>
+      <c r="I17" s="32"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
@@ -26192,17 +26691,17 @@
       <c r="X17" s="3"/>
     </row>
     <row r="18" spans="1:25" ht="16">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42" t="b">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="34"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="32"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
@@ -26220,17 +26719,17 @@
       <c r="X18" s="3"/>
     </row>
     <row r="19" spans="1:25" ht="16">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42" t="b">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
@@ -26248,17 +26747,17 @@
       <c r="X19" s="3"/>
     </row>
     <row r="20" spans="1:25" ht="16">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42" t="b">
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
@@ -26314,20 +26813,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>86</v>
       </c>
       <c r="K1" s="3"/>
@@ -38952,7 +39451,7 @@
       <c r="B752" s="3" t="s">
         <v>2258</v>
       </c>
-      <c r="C752" s="36" t="s">
+      <c r="C752" s="34" t="s">
         <v>2259</v>
       </c>
       <c r="D752" s="3" t="s">
@@ -66209,7 +66708,7 @@
       <c r="B2371" s="3" t="s">
         <v>6974</v>
       </c>
-      <c r="C2371" s="36" t="s">
+      <c r="C2371" s="34" t="s">
         <v>6975</v>
       </c>
       <c r="D2371" s="3" t="s">
@@ -66226,7 +66725,7 @@
       <c r="B2372" s="3" t="s">
         <v>6977</v>
       </c>
-      <c r="C2372" s="36" t="s">
+      <c r="C2372" s="34" t="s">
         <v>6978</v>
       </c>
       <c r="D2372" s="3" t="s">
@@ -68702,7 +69201,7 @@
       <c r="B2518" s="3" t="s">
         <v>7412</v>
       </c>
-      <c r="C2518" s="36" t="s">
+      <c r="C2518" s="34" t="s">
         <v>7413</v>
       </c>
       <c r="D2518" s="3" t="s">
@@ -68827,7 +69326,7 @@
     <row r="2535" spans="1:11" ht="15" customHeight="1">
       <c r="A2535" s="3"/>
       <c r="B2535" s="3"/>
-      <c r="C2535" s="36"/>
+      <c r="C2535" s="34"/>
       <c r="D2535" s="3"/>
       <c r="K2535" s="3"/>
     </row>
@@ -68869,10 +69368,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>7415</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>7416</v>
       </c>
       <c r="I1" s="3"/>
@@ -68891,7 +69390,7 @@
       <c r="V1" s="3"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3">
@@ -68913,8 +69412,8 @@
       <c r="V2" s="3"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A3" s="51" t="s">
-        <v>7547</v>
+      <c r="A3" s="49" t="s">
+        <v>7546</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -68932,7 +69431,7 @@
       <c r="V3" s="3"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="41" t="s">
         <v>7442</v>
       </c>
       <c r="B4" s="18">
@@ -68953,7 +69452,7 @@
       <c r="V4" s="3"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>7421</v>
       </c>
       <c r="B5" s="6">
@@ -68974,10 +69473,10 @@
       <c r="V5" s="3"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>7422</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>7</v>
       </c>
       <c r="C6" s="3"/>
@@ -68995,8 +69494,8 @@
       <c r="V6" s="3"/>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A7" s="53" t="s">
-        <v>7546</v>
+      <c r="A7" s="51" t="s">
+        <v>7545</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="3"/>
@@ -69014,8 +69513,8 @@
       <c r="V7" s="3"/>
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A8" s="51" t="s">
-        <v>7548</v>
+      <c r="A8" s="49" t="s">
+        <v>7547</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="3"/>
@@ -69033,8 +69532,8 @@
       <c r="V8" s="3"/>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A9" s="50" t="s">
-        <v>7535</v>
+      <c r="A9" s="48" t="s">
+        <v>7534</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -69052,10 +69551,10 @@
       <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>7420</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <v>2</v>
       </c>
       <c r="C10" s="3"/>
@@ -69073,10 +69572,10 @@
       <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>7423</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="20">
         <v>9</v>
       </c>
       <c r="C11" s="3"/>
@@ -69094,7 +69593,7 @@
       <c r="V11" s="3"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
         <v>7425</v>
       </c>
       <c r="B12" s="3">
@@ -69103,7 +69602,7 @@
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>7424</v>
       </c>
       <c r="B13" s="3">
@@ -69112,7 +69611,7 @@
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>7443</v>
       </c>
       <c r="B14" s="3">
@@ -69121,7 +69620,7 @@
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="20" t="s">
         <v>7427</v>
       </c>
       <c r="B15" s="3">
@@ -69130,7 +69629,7 @@
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>7428</v>
       </c>
       <c r="B16" s="3">
@@ -69139,7 +69638,7 @@
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="41" t="s">
         <v>7419</v>
       </c>
       <c r="B17" s="3">
@@ -69148,7 +69647,7 @@
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="20" t="s">
         <v>7440</v>
       </c>
       <c r="B18" s="3">
@@ -69157,7 +69656,7 @@
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="20" t="s">
         <v>7439</v>
       </c>
       <c r="B19" s="3">
@@ -69166,7 +69665,7 @@
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="20" t="s">
         <v>7429</v>
       </c>
       <c r="B20" s="3">
@@ -69175,7 +69674,7 @@
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="20" t="s">
         <v>7430</v>
       </c>
       <c r="B21" s="3">
@@ -69184,7 +69683,7 @@
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="20" t="s">
         <v>7441</v>
       </c>
       <c r="B22" s="3">
@@ -69193,7 +69692,7 @@
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="20" t="s">
         <v>7431</v>
       </c>
       <c r="B23" s="3">
@@ -69202,7 +69701,7 @@
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="20" t="s">
         <v>7432</v>
       </c>
       <c r="B24" s="3">
@@ -69211,7 +69710,7 @@
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="20" t="s">
         <v>7433</v>
       </c>
       <c r="B25" s="3">
@@ -69220,7 +69719,7 @@
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="20" t="s">
         <v>7434</v>
       </c>
       <c r="B26" s="3">
@@ -69229,7 +69728,7 @@
       <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="20" t="s">
         <v>7426</v>
       </c>
       <c r="B27" s="3">
@@ -69238,21 +69737,21 @@
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28" s="50" t="s">
-        <v>7541</v>
+      <c r="A28" s="48" t="s">
+        <v>7540</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A29" s="50" t="s">
-        <v>7536</v>
+      <c r="A29" s="48" t="s">
+        <v>7535</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="41" t="s">
         <v>7418</v>
       </c>
       <c r="B30" s="3">
@@ -69261,7 +69760,7 @@
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="20" t="s">
         <v>7435</v>
       </c>
       <c r="B31" s="3">
@@ -69270,7 +69769,7 @@
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="20" t="s">
         <v>7436</v>
       </c>
       <c r="B32" s="3">
@@ -69279,7 +69778,7 @@
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="20" t="s">
         <v>7438</v>
       </c>
       <c r="B33" s="3">
@@ -69288,7 +69787,7 @@
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="20" t="s">
         <v>7437</v>
       </c>
       <c r="B34" s="3">
@@ -69297,42 +69796,42 @@
       <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A35" s="50" t="s">
-        <v>7538</v>
+      <c r="A35" s="48" t="s">
+        <v>7537</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="50" t="s">
-        <v>7540</v>
+      <c r="A36" s="48" t="s">
+        <v>7539</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A37" s="50" t="s">
-        <v>7539</v>
+      <c r="A37" s="48" t="s">
+        <v>7538</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A38" s="50" t="s">
-        <v>7544</v>
+      <c r="A38" s="48" t="s">
+        <v>7543</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A39" s="50" t="s">
-        <v>7537</v>
+      <c r="A39" s="48" t="s">
+        <v>7536</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="41" t="s">
         <v>7417</v>
       </c>
       <c r="B40" s="3">
@@ -69341,22 +69840,22 @@
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A41" s="52" t="s">
-        <v>7545</v>
+      <c r="A41" s="50" t="s">
+        <v>7544</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A42" s="52" t="s">
-        <v>7543</v>
+      <c r="A42" s="50" t="s">
+        <v>7542</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A43" s="52" t="s">
-        <v>7542</v>
+      <c r="A43" s="50" t="s">
+        <v>7541</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -70904,10 +71403,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>7444</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>84</v>
       </c>
     </row>
@@ -70915,7 +71414,7 @@
       <c r="A2" s="3" t="s">
         <v>7445</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="36" t="s">
         <v>7446</v>
       </c>
     </row>
@@ -70931,7 +71430,7 @@
       <c r="A4" s="3" t="s">
         <v>7449</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>7450</v>
       </c>
     </row>
@@ -72005,22 +72504,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>7462</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="37" t="s">
         <v>7463</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>7464</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="37" t="s">
         <v>7465</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="37" t="s">
         <v>7466</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="37" t="s">
         <v>7467</v>
       </c>
     </row>
@@ -72031,16 +72530,16 @@
       <c r="B2" s="11" t="s">
         <v>7469</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="38" t="s">
         <v>7470</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="38" t="s">
         <v>7471</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>7472</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="38" t="s">
         <v>7473</v>
       </c>
     </row>
@@ -72051,16 +72550,16 @@
       <c r="B3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="38" t="s">
         <v>7475</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="44" t="s">
         <v>7476</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>7477</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="38" t="s">
         <v>7478</v>
       </c>
     </row>
@@ -72071,16 +72570,16 @@
       <c r="B4" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="38" t="s">
         <v>7480</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="38" t="s">
         <v>7481</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>7482</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="38" t="s">
         <v>7483</v>
       </c>
     </row>
@@ -72091,16 +72590,16 @@
       <c r="B5" s="11" t="s">
         <v>7485</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="38" t="s">
         <v>7486</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="38" t="s">
         <v>7487</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>7488</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="38" t="s">
         <v>7489</v>
       </c>
     </row>
@@ -72111,16 +72610,16 @@
       <c r="B6" s="11" t="s">
         <v>7490</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="38" t="s">
         <v>7491</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="38" t="s">
         <v>7492</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>7493</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="38" t="s">
         <v>7494</v>
       </c>
     </row>
@@ -72131,16 +72630,16 @@
       <c r="B7" s="11" t="s">
         <v>7495</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="38" t="s">
         <v>7496</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="38" t="s">
         <v>7497</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>7498</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="38" t="s">
         <v>7499</v>
       </c>
     </row>
@@ -72149,7 +72648,7 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="37"/>
+      <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
@@ -73223,21 +73722,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>7513</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="39" t="s">
         <v>7514</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="41"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -73247,7 +73746,7 @@
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="41"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -73257,9 +73756,9 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="41"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="36"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -73267,9 +73766,9 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="38"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -73277,9 +73776,9 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="41"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="38"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -73287,14 +73786,14 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="41"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="41"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -73322,9 +73821,9 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="41"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="38"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -73332,9 +73831,9 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="41"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="38"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -73342,7 +73841,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="41"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -73352,7 +73851,7 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="41"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -73362,7 +73861,7 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="41"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -73372,7 +73871,7 @@
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="41"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>

</xml_diff>

<commit_message>
Updated file with sequences for all of the TetR orthologs
</commit_message>
<xml_diff>
--- a/tetR Orthologs/tetR Orthologs.xlsx
+++ b/tetR Orthologs/tetR Orthologs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tracihaddock/Git/iGEM-distribution/tetR Orthologs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD49B14-9902-3440-956A-95AE415D89D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CD085F-D8FC-4A48-BD4F-56B9B49FCE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28900" yWindow="2180" windowWidth="37440" windowHeight="23840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33180" yWindow="-2400" windowWidth="37440" windowHeight="23840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7745" uniqueCount="7601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7785" uniqueCount="7617">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22759,9 +22759,6 @@
     <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/SrpR/1</t>
   </si>
   <si>
-    <t>not in SynBioHub</t>
-  </si>
-  <si>
     <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/QacR/1</t>
   </si>
   <si>
@@ -22907,6 +22904,57 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ttcgttaccaattgacagctagctATCATACCGCTATAATGGTATGTT</t>
+  </si>
+  <si>
+    <t>ttcgttaccaattgacagctAAACATACCGTGTGGTATGTTCtagc</t>
+  </si>
+  <si>
+    <t>not in SynBioHub; sequence pulled from the AddGene entry for the original plasmid</t>
+  </si>
+  <si>
+    <t>ttcGTGTCACTTTGACAGCAGTGTCACtcctaggtataatgctagc</t>
+  </si>
+  <si>
+    <t>ttcgttaccaattgacaCTAGACCGGTCTGTCTAtataatgctagc</t>
+  </si>
+  <si>
+    <t>ttcgttaccaattgacaCTAACTGACGGTTCAGTTAGgttgctagctactagagaaagaggagaaatactagatggtgagccgtcaattgtctgattcgttaccaattgacactaactgctgttcagttaggttgctagc</t>
+  </si>
+  <si>
+    <t>ttcgttaccaattgacagctagctcTTATTGATTTTTAATCAAATAA</t>
+  </si>
+  <si>
+    <t>http://www.addgene.org/49360/sequences/</t>
+  </si>
+  <si>
+    <t>ttcgttaccaattgacATATTTAAAATTCTTGTTTAAAatgctagc</t>
+  </si>
+  <si>
+    <t>http://www.addgene.org/49361/sequences/</t>
+  </si>
+  <si>
+    <t>ttcgttaccaattgacaTTATTGATAAATCTGCGTAAAATgctagc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.addgene.org/49371/sequences/ </t>
+  </si>
+  <si>
+    <t>http://www.addgene.org/49373/sequences/</t>
+  </si>
+  <si>
+    <t>http://www.addgene.org/49370/sequences/</t>
+  </si>
+  <si>
+    <t>http://www.addgene.org/49359/sequences/</t>
+  </si>
+  <si>
+    <t>http://www.addgene.org/49365/sequences/</t>
+  </si>
+  <si>
+    <t>http://www.addgene.org/49366/sequences/</t>
   </si>
 </sst>
 </file>
@@ -23282,7 +23330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23358,6 +23406,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -23819,7 +23868,7 @@
   <dimension ref="A1:M982"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24213,7 +24262,7 @@
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="65" t="s">
+      <c r="G17" s="66" t="s">
         <v>7550</v>
       </c>
       <c r="H17" s="63" t="s">
@@ -24242,7 +24291,7 @@
         <v>47</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>7592</v>
+        <v>7591</v>
       </c>
       <c r="D18" s="64"/>
       <c r="E18" s="63"/>
@@ -24265,7 +24314,7 @@
         <v>663</v>
       </c>
       <c r="M18" s="62" t="s">
-        <v>7591</v>
+        <v>7590</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24280,7 +24329,7 @@
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="52" t="s">
-        <v>7552</v>
+        <v>7551</v>
       </c>
       <c r="H19" s="18" t="s">
         <v>7537</v>
@@ -24302,7 +24351,7 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="40" t="s">
-        <v>7560</v>
+        <v>7559</v>
       </c>
       <c r="B20" s="40" t="s">
         <v>47</v>
@@ -24312,7 +24361,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="20" t="s">
-        <v>7559</v>
+        <v>7558</v>
       </c>
       <c r="H20" s="18" t="s">
         <v>7537</v>
@@ -24340,7 +24389,7 @@
         <v>47</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>7592</v>
+        <v>7591</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="18"/>
@@ -24362,8 +24411,8 @@
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M21,CHAR(160)," ")," ",""))))</f>
         <v>648</v>
       </c>
-      <c r="M21" s="66" t="s">
-        <v>7593</v>
+      <c r="M21" s="67" t="s">
+        <v>7592</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24374,7 +24423,7 @@
         <v>47</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>7592</v>
+        <v>7591</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
@@ -24396,8 +24445,8 @@
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M22,CHAR(160)," ")," ",""))))</f>
         <v>807</v>
       </c>
-      <c r="M22" s="66" t="s">
-        <v>7594</v>
+      <c r="M22" s="67" t="s">
+        <v>7593</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24412,7 +24461,7 @@
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="18" t="s">
-        <v>7563</v>
+        <v>7562</v>
       </c>
       <c r="H23" s="18" t="s">
         <v>7540</v>
@@ -24440,7 +24489,7 @@
         <v>47</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>7592</v>
+        <v>7591</v>
       </c>
       <c r="D24" s="64"/>
       <c r="E24" s="63"/>
@@ -24462,8 +24511,8 @@
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M24,CHAR(160)," ")," ",""))))</f>
         <v>618</v>
       </c>
-      <c r="M24" s="66" t="s">
-        <v>7595</v>
+      <c r="M24" s="67" t="s">
+        <v>7594</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24474,7 +24523,7 @@
         <v>47</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>7592</v>
+        <v>7591</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="18"/>
@@ -24496,8 +24545,8 @@
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M25,CHAR(160)," ")," ",""))))</f>
         <v>642</v>
       </c>
-      <c r="M25" s="66" t="s">
-        <v>7596</v>
+      <c r="M25" s="67" t="s">
+        <v>7595</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24512,7 +24561,7 @@
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="52" t="s">
-        <v>7566</v>
+        <v>7565</v>
       </c>
       <c r="H26" s="63" t="s">
         <v>7535</v>
@@ -24544,7 +24593,7 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="52" t="s">
-        <v>7569</v>
+        <v>7568</v>
       </c>
       <c r="H27" s="18" t="s">
         <v>7419</v>
@@ -24576,7 +24625,7 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="52" t="s">
-        <v>7572</v>
+        <v>7571</v>
       </c>
       <c r="H28" s="18" t="s">
         <v>7542</v>
@@ -24604,7 +24653,7 @@
         <v>47</v>
       </c>
       <c r="C29" s="40" t="s">
-        <v>7592</v>
+        <v>7591</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="18"/>
@@ -24626,8 +24675,8 @@
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M29,CHAR(160)," ")," ",""))))</f>
         <v>870</v>
       </c>
-      <c r="M29" s="66" t="s">
-        <v>7597</v>
+      <c r="M29" s="67" t="s">
+        <v>7596</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24638,7 +24687,7 @@
         <v>47</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>7592</v>
+        <v>7591</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="18"/>
@@ -24660,8 +24709,8 @@
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M30,CHAR(160)," ")," ",""))))</f>
         <v>612</v>
       </c>
-      <c r="M30" s="66" t="s">
-        <v>7599</v>
+      <c r="M30" s="67" t="s">
+        <v>7598</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24672,7 +24721,7 @@
         <v>47</v>
       </c>
       <c r="C31" s="40" t="s">
-        <v>7592</v>
+        <v>7591</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="18"/>
@@ -24694,8 +24743,8 @@
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M31,CHAR(160)," ")," ",""))))</f>
         <v>636</v>
       </c>
-      <c r="M31" s="66" t="s">
-        <v>7598</v>
+      <c r="M31" s="67" t="s">
+        <v>7597</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24709,8 +24758,8 @@
       <c r="D32" s="64"/>
       <c r="E32" s="63"/>
       <c r="F32" s="63"/>
-      <c r="G32" s="65" t="s">
-        <v>7575</v>
+      <c r="G32" s="66" t="s">
+        <v>7574</v>
       </c>
       <c r="H32" s="63" t="s">
         <v>7546</v>
@@ -24742,7 +24791,7 @@
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="52" t="s">
-        <v>7578</v>
+        <v>7577</v>
       </c>
       <c r="H33" s="18" t="s">
         <v>7547</v>
@@ -24794,7 +24843,7 @@
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="40" t="s">
-        <v>7553</v>
+        <v>7552</v>
       </c>
       <c r="B35" s="40" t="s">
         <v>41</v>
@@ -24804,7 +24853,7 @@
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="52" t="s">
-        <v>7554</v>
+        <v>7553</v>
       </c>
       <c r="H35" s="63" t="s">
         <v>7537</v>
@@ -24826,19 +24875,19 @@
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="40" t="s">
-        <v>7555</v>
+        <v>7554</v>
       </c>
       <c r="B36" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>7600</v>
+        <v>7599</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="20" t="s">
-        <v>7556</v>
+        <v>7555</v>
       </c>
       <c r="H36" s="18" t="s">
         <v>7443</v>
@@ -24860,7 +24909,7 @@
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="40" t="s">
-        <v>7557</v>
+        <v>7556</v>
       </c>
       <c r="B37" s="40" t="s">
         <v>41</v>
@@ -24870,7 +24919,7 @@
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
       <c r="G37" s="20" t="s">
-        <v>7558</v>
+        <v>7557</v>
       </c>
       <c r="H37" s="18" t="s">
         <v>7535</v>
@@ -24892,7 +24941,7 @@
     </row>
     <row r="38" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="40" t="s">
-        <v>7561</v>
+        <v>7560</v>
       </c>
       <c r="B38" s="40" t="s">
         <v>41</v>
@@ -24902,7 +24951,7 @@
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="20" t="s">
-        <v>7562</v>
+        <v>7561</v>
       </c>
       <c r="H38" s="48" t="s">
         <v>7537</v>
@@ -24924,7 +24973,7 @@
     </row>
     <row r="39" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="40" t="s">
-        <v>7564</v>
+        <v>7563</v>
       </c>
       <c r="B39" s="40" t="s">
         <v>41</v>
@@ -24934,7 +24983,7 @@
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="52" t="s">
-        <v>7565</v>
+        <v>7564</v>
       </c>
       <c r="H39" s="53" t="s">
         <v>7540</v>
@@ -24956,7 +25005,7 @@
     </row>
     <row r="40" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="40" t="s">
-        <v>7567</v>
+        <v>7566</v>
       </c>
       <c r="B40" s="40" t="s">
         <v>41</v>
@@ -24966,7 +25015,7 @@
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="52" t="s">
-        <v>7568</v>
+        <v>7567</v>
       </c>
       <c r="H40" s="48" t="s">
         <v>7535</v>
@@ -24988,7 +25037,7 @@
     </row>
     <row r="41" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="40" t="s">
-        <v>7570</v>
+        <v>7569</v>
       </c>
       <c r="B41" s="40" t="s">
         <v>41</v>
@@ -24998,7 +25047,7 @@
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="52" t="s">
-        <v>7571</v>
+        <v>7570</v>
       </c>
       <c r="H41" s="53" t="s">
         <v>7419</v>
@@ -25020,7 +25069,7 @@
     </row>
     <row r="42" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="40" t="s">
-        <v>7573</v>
+        <v>7572</v>
       </c>
       <c r="B42" s="40" t="s">
         <v>41</v>
@@ -25030,7 +25079,7 @@
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="52" t="s">
-        <v>7574</v>
+        <v>7573</v>
       </c>
       <c r="H42" s="48" t="s">
         <v>7542</v>
@@ -25052,7 +25101,7 @@
     </row>
     <row r="43" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="40" t="s">
-        <v>7576</v>
+        <v>7575</v>
       </c>
       <c r="B43" s="40" t="s">
         <v>41</v>
@@ -25062,7 +25111,7 @@
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="52" t="s">
-        <v>7577</v>
+        <v>7576</v>
       </c>
       <c r="H43" s="48" t="s">
         <v>7546</v>
@@ -25084,7 +25133,7 @@
     </row>
     <row r="44" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="40" t="s">
-        <v>7579</v>
+        <v>7578</v>
       </c>
       <c r="B44" s="40" t="s">
         <v>41</v>
@@ -25094,7 +25143,7 @@
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="52" t="s">
-        <v>7580</v>
+        <v>7579</v>
       </c>
       <c r="H44" s="53" t="s">
         <v>7547</v>
@@ -25116,20 +25165,28 @@
     </row>
     <row r="45" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="40" t="s">
-        <v>7581</v>
+        <v>7580</v>
       </c>
       <c r="B45" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>7551</v>
+        <v>7602</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
+      <c r="F45" s="49" t="s">
+        <v>7485</v>
+      </c>
+      <c r="G45" s="52" t="s">
+        <v>7612</v>
+      </c>
+      <c r="H45" s="63" t="s">
+        <v>7536</v>
+      </c>
+      <c r="I45" s="63" t="s">
+        <v>7419</v>
+      </c>
       <c r="J45" s="18" t="b">
         <v>0</v>
       </c>
@@ -25138,26 +25195,36 @@
       </c>
       <c r="L45" s="15">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M45,CHAR(160)," ")," ",""))))</f>
-        <v>0</v>
-      </c>
-      <c r="M45" s="49"/>
+        <v>46</v>
+      </c>
+      <c r="M45" s="49" t="s">
+        <v>7601</v>
+      </c>
     </row>
     <row r="46" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="40" t="s">
-        <v>7582</v>
+        <v>7581</v>
       </c>
       <c r="B46" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>7551</v>
+        <v>7602</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
+      <c r="F46" s="49" t="s">
+        <v>7485</v>
+      </c>
+      <c r="G46" s="52" t="s">
+        <v>7613</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>7538</v>
+      </c>
+      <c r="I46" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J46" s="18" t="b">
         <v>0</v>
       </c>
@@ -25166,26 +25233,36 @@
       </c>
       <c r="L46" s="15">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M46,CHAR(160)," ")," ",""))))</f>
-        <v>0</v>
-      </c>
-      <c r="M46" s="49"/>
+        <v>48</v>
+      </c>
+      <c r="M46" s="49" t="s">
+        <v>7600</v>
+      </c>
     </row>
     <row r="47" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="40" t="s">
-        <v>7583</v>
+        <v>7582</v>
       </c>
       <c r="B47" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>7551</v>
+        <v>7602</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
+      <c r="F47" s="49" t="s">
+        <v>7485</v>
+      </c>
+      <c r="G47" s="52" t="s">
+        <v>7614</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>7539</v>
+      </c>
+      <c r="I47" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J47" s="18" t="b">
         <v>0</v>
       </c>
@@ -25194,26 +25271,36 @@
       </c>
       <c r="L47" s="15">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M47,CHAR(160)," ")," ",""))))</f>
-        <v>0</v>
-      </c>
-      <c r="M47" s="49"/>
+        <v>46</v>
+      </c>
+      <c r="M47" s="49" t="s">
+        <v>7603</v>
+      </c>
     </row>
     <row r="48" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="40" t="s">
-        <v>7584</v>
+        <v>7583</v>
       </c>
       <c r="B48" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>7551</v>
+        <v>7602</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
+      <c r="F48" s="49" t="s">
+        <v>7485</v>
+      </c>
+      <c r="G48" s="52" t="s">
+        <v>7615</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>7443</v>
+      </c>
+      <c r="I48" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J48" s="18" t="b">
         <v>0</v>
       </c>
@@ -25222,26 +25309,36 @@
       </c>
       <c r="L48" s="15">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M48,CHAR(160)," ")," ",""))))</f>
-        <v>0</v>
-      </c>
-      <c r="M48" s="49"/>
+        <v>46</v>
+      </c>
+      <c r="M48" s="49" t="s">
+        <v>7604</v>
+      </c>
     </row>
     <row r="49" spans="1:13" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="57" t="s">
-        <v>7585</v>
+        <v>7584</v>
       </c>
       <c r="B49" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>7551</v>
+        <v>7602</v>
       </c>
       <c r="D49" s="59"/>
       <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="59"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
+      <c r="F49" s="49" t="s">
+        <v>7485</v>
+      </c>
+      <c r="G49" s="65" t="s">
+        <v>7616</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>7543</v>
+      </c>
+      <c r="I49" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J49" s="58" t="b">
         <v>0</v>
       </c>
@@ -25250,26 +25347,36 @@
       </c>
       <c r="L49" s="15">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M49,CHAR(160)," ")," ",""))))</f>
-        <v>0</v>
-      </c>
-      <c r="M49" s="60"/>
+        <v>140</v>
+      </c>
+      <c r="M49" s="60" t="s">
+        <v>7605</v>
+      </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="49" t="s">
-        <v>7586</v>
+        <v>7585</v>
       </c>
       <c r="B50" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>7551</v>
+        <v>7602</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
+      <c r="F50" s="49" t="s">
+        <v>7485</v>
+      </c>
+      <c r="G50" s="65" t="s">
+        <v>7607</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>7544</v>
+      </c>
+      <c r="I50" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J50" s="58" t="b">
         <v>0</v>
       </c>
@@ -25278,26 +25385,36 @@
       </c>
       <c r="L50" s="15">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M50,CHAR(160)," ")," ",""))))</f>
-        <v>0</v>
-      </c>
-      <c r="M50" s="49"/>
+        <v>47</v>
+      </c>
+      <c r="M50" s="49" t="s">
+        <v>7606</v>
+      </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="60" t="s">
-        <v>7587</v>
+        <v>7586</v>
       </c>
       <c r="B51" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>7551</v>
+        <v>7602</v>
       </c>
       <c r="D51" s="61"/>
       <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
+      <c r="F51" s="60" t="s">
+        <v>7485</v>
+      </c>
+      <c r="G51" s="65" t="s">
+        <v>7609</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>7545</v>
+      </c>
+      <c r="I51" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J51" s="58" t="b">
         <v>0</v>
       </c>
@@ -25306,23 +25423,34 @@
       </c>
       <c r="L51" s="15">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M51,CHAR(160)," ")," ",""))))</f>
-        <v>0</v>
-      </c>
-      <c r="M51" s="60"/>
+        <v>46</v>
+      </c>
+      <c r="M51" s="60" t="s">
+        <v>7608</v>
+      </c>
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="49" t="s">
-        <v>7590</v>
+        <v>7589</v>
       </c>
       <c r="B52" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>7551</v>
-      </c>
-      <c r="G52" s="59"/>
-      <c r="H52" s="58"/>
-      <c r="I52" s="58"/>
+        <v>7602</v>
+      </c>
+      <c r="F52" s="49" t="s">
+        <v>7485</v>
+      </c>
+      <c r="G52" s="65" t="s">
+        <v>7611</v>
+      </c>
+      <c r="H52" s="63" t="s">
+        <v>7541</v>
+      </c>
+      <c r="I52" s="63" t="s">
+        <v>7419</v>
+      </c>
       <c r="J52" s="58" t="b">
         <v>0</v>
       </c>
@@ -25331,9 +25459,11 @@
       </c>
       <c r="L52" s="15">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M52,CHAR(160)," ")," ",""))))</f>
-        <v>0</v>
-      </c>
-      <c r="M52" s="49"/>
+        <v>46</v>
+      </c>
+      <c r="M52" s="49" t="s">
+        <v>7610</v>
+      </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26286,11 +26416,19 @@
     <hyperlink ref="G43" r:id="rId14" xr:uid="{DAF6E551-6F9D-D044-9AE2-23760AE41E3D}"/>
     <hyperlink ref="G33" r:id="rId15" xr:uid="{38243E19-8216-9446-8B60-4C042B14C971}"/>
     <hyperlink ref="G44" r:id="rId16" xr:uid="{73B69518-BD7D-554E-9756-E4CBB2D815B4}"/>
+    <hyperlink ref="G50" r:id="rId17" xr:uid="{8D1EDE18-0DF0-8746-8F56-39CE95B38FAC}"/>
+    <hyperlink ref="G51" r:id="rId18" xr:uid="{6D7C090B-3768-E946-B6F6-043048920F25}"/>
+    <hyperlink ref="G52" r:id="rId19" xr:uid="{7B219E1E-9AEB-A14C-BFCF-23B46E2613D5}"/>
+    <hyperlink ref="G45" r:id="rId20" xr:uid="{4B5CAA43-4BB3-3143-AA32-3F3AAFC0079C}"/>
+    <hyperlink ref="G46" r:id="rId21" xr:uid="{ADE31EBE-B445-EE47-B5E2-65EF210146E5}"/>
+    <hyperlink ref="G47" r:id="rId22" xr:uid="{D8593484-0B24-184E-B4A9-459ACDE13EDC}"/>
+    <hyperlink ref="G48" r:id="rId23" xr:uid="{E78823C4-B413-664F-8854-26778751C315}"/>
+    <hyperlink ref="G49" r:id="rId24" xr:uid="{84CC214C-4997-C443-AAD7-9BDA34BD2ABF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId25"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -26299,7 +26437,7 @@
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F49</xm:sqref>
+          <xm:sqref>F15:F44</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -26836,7 +26974,7 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="49" t="s">
-        <v>7589</v>
+        <v>7588</v>
       </c>
       <c r="B14" s="21"/>
       <c r="D14" s="21" t="b">
@@ -26847,7 +26985,7 @@
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="49" t="s">
-        <v>7588</v>
+        <v>7587</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="31"/>

</xml_diff>

<commit_message>
Fix incorrect "final product" marks in 2A peptides and tetR orthologs Patch issue affecting export of OpenYeast - note that OpenYeast is appearing in FASTA and shouldn't be, however
</commit_message>
<xml_diff>
--- a/tetR Orthologs/tetR Orthologs.xlsx
+++ b/tetR Orthologs/tetR Orthologs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/tetR Orthologs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B6BAB3-178F-0442-80A7-6A83C4A6620C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5065E082-7122-294A-B396-27640E8F1EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="1000" windowWidth="33660" windowHeight="21060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ontology Terms'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Organism Terms'!$A$1:$B$1000</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -26236,7 +26236,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26552,7 +26552,7 @@
         <v>7622</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="40" t="s">
         <v>102</v>
@@ -26567,7 +26567,7 @@
         <v>7621</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="40" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
working on replacing original tetR file due to loss of form validation
</commit_message>
<xml_diff>
--- a/tetR Orthologs/tetR Orthologs.xlsx
+++ b/tetR Orthologs/tetR Orthologs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/tetR Orthologs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/tetR Orthologs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5065E082-7122-294A-B396-27640E8F1EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E70C8F-682F-7D4C-8BFC-07EC6EB4A6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1000" windowWidth="33660" windowHeight="21060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35380" yWindow="-2000" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ontology Terms'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Organism Terms'!$A$1:$B$1000</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7825" uniqueCount="7625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7825" uniqueCount="7626">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22905,6 +22905,9 @@
   </si>
   <si>
     <t>pQacR, pAmtR, pSrpR, pIcaRA, pPhlF, pPsrA, pBetI, pLitR, pAmeR, pBM3R1, pTarA, pScbR, pSmcR, pButR, pMcbR, pOrf2, pHapR, pHlyllR</t>
+  </si>
+  <si>
+    <t>pSB1C5</t>
   </si>
 </sst>
 </file>
@@ -23782,8 +23785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M982"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77:C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24631,23 +24634,23 @@
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="40" t="s">
-        <v>102</v>
+        <v>7625</v>
       </c>
       <c r="B34" s="40" t="s">
         <v>103</v>
       </c>
       <c r="D34" s="42"/>
       <c r="F34" t="s">
-        <v>8</v>
+        <v>7617</v>
       </c>
       <c r="G34" s="42" t="s">
-        <v>102</v>
+        <v>7625</v>
       </c>
       <c r="J34" t="b">
         <v>0</v>
       </c>
       <c r="K34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34" s="12">
         <v>0</v>
@@ -26235,7 +26238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixing missing comma in tetR Orthologs
</commit_message>
<xml_diff>
--- a/tetR Orthologs/tetR Orthologs.xlsx
+++ b/tetR Orthologs/tetR Orthologs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/tetR Orthologs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9105194E-5190-FA49-81C7-4C4638685111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816B3C17-C0CF-6449-8063-BAF1CE144ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="500" windowWidth="28800" windowHeight="13240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -23049,15 +23049,9 @@
     <t>pAmtR, pPsrA, pAmeR, pScbR, pSmcR, pButR, pOrf2, pHapR, pHlyllR</t>
   </si>
   <si>
-    <t>pQacR, pIcaRA, pLitR, pPhlF, pMcbR pBetI, pTarA, pSrpR, pBM3R1</t>
-  </si>
-  <si>
     <t>LitR, BM3R1, IcaRA</t>
   </si>
   <si>
-    <t>pQacR, pIcaRA, pPhlF, pMcbR pBetI, pTarA, pSrpR, pBM3R1</t>
-  </si>
-  <si>
     <t>Unable to build Promoters</t>
   </si>
   <si>
@@ -23080,6 +23074,12 @@
   </si>
   <si>
     <t>Synthesized as linear fragments and cloned into pSB1C3</t>
+  </si>
+  <si>
+    <t>pQacR, pIcaRA, pPhlF, pMcbR, pBetI, pTarA, pSrpR, pBM3R1</t>
+  </si>
+  <si>
+    <t>pQacR, pIcaRA, pLitR, pPhlF, pMcbR, pBetI, pTarA, pSrpR, pBM3R1</t>
   </si>
 </sst>
 </file>
@@ -23498,12 +23498,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23960,8 +23960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView topLeftCell="C39" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24035,12 +24035,12 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="55"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="56"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -26857,8 +26857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -27366,7 +27366,7 @@
         <v>7533</v>
       </c>
       <c r="H14" s="52" t="s">
-        <v>7656</v>
+        <v>7654</v>
       </c>
       <c r="I14" s="51" t="s">
         <v>7534</v>
@@ -27431,10 +27431,10 @@
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" s="50" t="s">
-        <v>7651</v>
-      </c>
-      <c r="B16" s="56" t="s">
-        <v>7657</v>
+        <v>7649</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>7655</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="22" t="b">
@@ -27451,7 +27451,7 @@
         <v>7635</v>
       </c>
       <c r="I16" s="51" t="s">
-        <v>7648</v>
+        <v>7658</v>
       </c>
       <c r="J16" s="18" t="s">
         <v>7636</v>
@@ -27475,10 +27475,10 @@
     </row>
     <row r="17" spans="1:25" ht="15" customHeight="1">
       <c r="A17" s="42" t="s">
-        <v>7652</v>
-      </c>
-      <c r="B17" s="56" t="s">
-        <v>7657</v>
+        <v>7650</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>7655</v>
       </c>
       <c r="C17" s="41"/>
       <c r="D17" s="22" t="b">
@@ -27492,7 +27492,7 @@
         <v>7533</v>
       </c>
       <c r="H17" s="52" t="s">
-        <v>7655</v>
+        <v>7653</v>
       </c>
       <c r="I17" s="51" t="s">
         <v>7534</v>
@@ -27515,10 +27515,10 @@
     </row>
     <row r="18" spans="1:25" ht="17">
       <c r="A18" s="42" t="s">
-        <v>7654</v>
-      </c>
-      <c r="B18" s="56" t="s">
-        <v>7658</v>
+        <v>7652</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>7656</v>
       </c>
       <c r="C18" s="41"/>
       <c r="D18" s="22" t="b">
@@ -27532,7 +27532,7 @@
         <v>7533</v>
       </c>
       <c r="H18" s="52" t="s">
-        <v>7649</v>
+        <v>7648</v>
       </c>
       <c r="I18" s="51" t="s">
         <v>7534</v>
@@ -27555,10 +27555,10 @@
     </row>
     <row r="19" spans="1:25" ht="16">
       <c r="A19" s="42" t="s">
-        <v>7653</v>
-      </c>
-      <c r="B19" s="56" t="s">
-        <v>7658</v>
+        <v>7651</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>7656</v>
       </c>
       <c r="C19" s="41"/>
       <c r="D19" s="22" t="b">
@@ -27575,7 +27575,7 @@
         <v>7635</v>
       </c>
       <c r="I19" s="42" t="s">
-        <v>7650</v>
+        <v>7657</v>
       </c>
       <c r="J19" s="18" t="s">
         <v>7636</v>

</xml_diff>